<commit_message>
effect of capital letters features
</commit_message>
<xml_diff>
--- a/experiments/capital/bert-base-cased_15/123/incorrect_predictions.xlsx
+++ b/experiments/capital/bert-base-cased_15/123/incorrect_predictions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,21 +462,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AirSense communication error . Unable to display nearby manned aircraft and anti-collision warnings . Fly with caution .</t>
+          <t>Aircraft ActiveTrack available at max speed . Obstacle Avoidance is not available .</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Unable to display nearby manned aircraft and anti-collision warnings</t>
+          <t>Aircraft ActiveTrack available at max speed</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4-12</t>
+          <t>0-5</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -487,21 +487,21 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Approaching a No-Fly Zone . RTH may be affected . Fly with caution .</t>
+          <t>Aircraft ActiveTrack available at max speed . When exceeding nnn, Obstacle Avoidance is not available .</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RTH may be affected</t>
+          <t>Aircraft ActiveTrack available at max speed</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>5-8</t>
+          <t>0-5</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -512,21 +512,21 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Compass error , calibration required .</t>
+          <t>Aircraft ActiveTrack available at max speed . When exceeding nnn, Obstacle Avoidance is not available .</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>calibration required</t>
+          <t>When exceeding nnn, Obstacle Avoidance is not available</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>7-14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -537,99 +537,449 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Error: Course angle control error . Please ensure the propellers are installed on the correct motors .</t>
+          <t>Aircraft ActiveTrack available at max speed . When exceeding nnn, Obstacle Avoidance is not available .</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Error: Course angle control error</t>
+          <t>When exceeding nnn,</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0-4</t>
+          <t>7-9</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Error: Course angle control error . Please ensure the propellers are installed on the correct motors .</t>
+          <t>Check whether propellers are installed correctly . If the propellers are installed correctly and the aircraft still cannot takeoff, a motor error may exist . Contact DJI Support for assistance .</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Course angle control error</t>
+          <t>If the propellers are installed correctly and the aircraft still cannot takeoff, a motor error may exist</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1-4</t>
+          <t>7-23</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Missing</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>IMU warming up . Wait before taking off .</t>
+          <t>Check whether propellers are installed correctly . If the propellers are installed correctly and the aircraft still cannot takeoff, a motor error may exist . Contact DJI Support for assistance .</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>IMU warming up</t>
+          <t>If the propellers are installed correctly and the aircraft still cannot takeoff,</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>7-18</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Missing</t>
+          <t>False</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>IMU warming up . Wait before taking off .</t>
+          <t>Compass abnormal . Solution: 1. Ensure there are no magnets or metal objects near the aircraft . The ground or walls may contain metal . Move away from sources of interference before attempting flight . 2. Calibrate Compass Before Takeoff .</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>IMU warming</t>
+          <t>2. Calibrate Compass Before Takeoff</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>35-39</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>50</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Compass abnormal . Solution: 1. Ensure there are no magnets or metal objects near the aircraft . The ground or walls may contain metal . Move away from sources of interference before attempting flight . 2. Calibrate Compass Before Takeoff .</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Calibrate Compass Before Takeoff</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>36-39</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>66</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Downlink data connection lost for nnn seconds .</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Downlink data connection lost for nnn seconds</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0-6</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>66</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Downlink data connection lost for nnn seconds .</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Downlink data connection lost for nnn</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0-5</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>70</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Downward ambient light too low . Obstacle avoidance unavailable . Fly with caution . Backward ambient light too low . Backward obstacle avoidance unavailable . Only infrared sensors available . Fly with caution .</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Backward ambient light too low</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>14-18</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>77</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Exiting GPS mode : Unknown Error .</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Unknown Error</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4-5</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>81</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Extra payload detected . Return aircraft to an area nearby the home point promptly and fly in a wind-free environment to ensure flight safety .</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Return aircraft to an area nearby the home point promptly and fly in a wind-free environment to ensure flight safety</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4-23</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>86</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Flight altitude exceeds nnn . May violate local policies and regulations . Ensure you have obtained proper airspace authorization .</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>May violate local policies and regulations</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>5-10</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>91</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>GEO Zone Info: The target area is in an Altitude Zone . Flight altitude restricted to nnn .</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>GEO Zone Info: The target area is in an Altitude Zone</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0-10</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>91</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>GEO Zone Info: The target area is in an Altitude Zone . Flight altitude restricted to nnn .</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>GEO Zone Info:</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0-2</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>91</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>GEO Zone Info: The target area is in an Altitude Zone . Flight altitude restricted to nnn .</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>The target area is in an Altitude Zone</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>3-10</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>113</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Insufficient SD card space . Change card or delete files .</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Insufficient SD card space</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0-3</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>115</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Landin .</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Landin</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0-0</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>147</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SD card write speed is too slow . Not suitable for shooting a 4K video .</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Not suitable for shooting a 4K video</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>8-14</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>147</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SD card write speed is too slow . Not suitable for shooting a 4K video .</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Not suitable for shooting a 4K</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>8-13</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>False</t>
         </is>

</xml_diff>